<commit_message>
Add more sheets in data.xlsx Using data focus on rows not column. For me, this way is vary helpful when used test suite
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94244CA8-181B-42E7-987A-178D0BB044A5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06343DD-DD5A-4E12-9B96-A2657E773FAB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="3" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="SaldeOrder" sheetId="5" r:id="rId4"/>
     <sheet name="Mydata" sheetId="4" r:id="rId5"/>
     <sheet name="adminRole" sheetId="6" r:id="rId6"/>
+    <sheet name="userRole" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -162,50 +163,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Garden, Papaya</t>
-  </si>
-  <si>
-    <t>20,120 THB</t>
-  </si>
-  <si>
-    <t>Banana, Garden, Banana, Rambutan</t>
-  </si>
-  <si>
-    <t>60,570 THB</t>
-  </si>
-  <si>
-    <t>Garden, Banana, Orange, Papaya, Rambutan</t>
-  </si>
-  <si>
-    <t>21,288 THB</t>
-  </si>
-  <si>
-    <t>41,750 THB</t>
-  </si>
-  <si>
-    <t>41,288 THB</t>
-  </si>
-  <si>
-    <t>20,462 THB</t>
-  </si>
-  <si>
-    <t>60,462 THB</t>
-  </si>
-  <si>
-    <r>
-      <t>Total price: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF212529"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>307,690 THB</t>
-    </r>
-  </si>
-  <si>
     <t>SaleOrderId</t>
   </si>
   <si>
@@ -222,6 +179,18 @@
   </si>
   <si>
     <t>t003,t004,t005,t006</t>
+  </si>
+  <si>
+    <t>Transaction List</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t>data3</t>
   </si>
 </sst>
 </file>
@@ -253,8 +222,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="18"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -285,8 +253,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -629,7 +599,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,27 +916,27 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>59</v>
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>61</v>
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -976,10 +946,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5A8D0-6A69-4317-BF67-BDCA8742CFBC}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,253 +958,42 @@
     <col min="2" max="2" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>55</v>
-      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1246,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D612F2-3354-4190-80F9-B642323BDC9B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,4 +1030,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC93449-C4A4-4C07-A832-0375A4BBE05D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>